<commit_message>
- QR Sample Scans - Meeting recording
</commit_message>
<xml_diff>
--- a/qrbarcode scans.xlsx
+++ b/qrbarcode scans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickylenon/PROJECTX/qrbarcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1636AE46-53BD-8E4F-887B-A396FA322ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB805F2-5446-5240-8456-82A2156E6F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{07329640-7ECA-384A-9609-484D1E397277}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21860" xr2:uid="{07329640-7ECA-384A-9609-484D1E397277}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
   <si>
     <t>015 24112620409</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>CBM-205624</t>
+  </si>
+  <si>
+    <t>3A951-59S00_241127-01k</t>
   </si>
 </sst>
 </file>
@@ -101,10 +104,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -133,8 +142,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1231900</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>254000</xdr:rowOff>
     </xdr:to>
@@ -176,8 +185,8 @@
       <xdr:rowOff>482600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>515724</xdr:rowOff>
     </xdr:to>
@@ -204,6 +213,50 @@
         <a:xfrm>
           <a:off x="2743200" y="8864600"/>
           <a:ext cx="7772400" cy="2319124"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>203332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>847495</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D7B0C6F-1485-F82D-4944-CAD09F9161A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2705100" y="13919332"/>
+          <a:ext cx="14325600" cy="3692163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -532,15 +585,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2762419C-1BED-9641-A29C-170436E1AC94}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="400" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.6640625" style="1" customWidth="1"/>
+    <col min="2" max="19" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -608,6 +662,137 @@
         <v>200</v>
       </c>
     </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" s="3" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>